<commit_message>
Ajuste de detalles en modulos
</commit_message>
<xml_diff>
--- a/winAsimilados/Resources/Formato_Masivo_Info_Caratula17.xlsx
+++ b/winAsimilados/Resources/Formato_Masivo_Info_Caratula17.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aespejel\source\repos\winAsimilados\winAsimilados\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65C96F4-A35D-4851-836B-0339D24BFD2D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03F2A01-2C77-456C-A186-497DB2956A1E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{7D684382-455D-490A-8956-2EC1B8E2E487}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7D684382-455D-490A-8956-2EC1B8E2E487}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
   <si>
     <t># Empleado</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Quincenal</t>
+  </si>
+  <si>
+    <t>Mensual</t>
   </si>
 </sst>
 </file>
@@ -461,7 +464,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,10 +495,10 @@
         <v>320</v>
       </c>
       <c r="B3" s="6">
-        <v>4785.8500000000004</v>
+        <v>22785.85</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" s="3"/>
     </row>
@@ -504,10 +507,10 @@
         <v>321</v>
       </c>
       <c r="B4" s="6">
-        <v>5720.09</v>
+        <v>17720.09</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" s="3"/>
     </row>
@@ -519,7 +522,7 @@
         <v>23031.31</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" s="3"/>
     </row>
@@ -528,10 +531,10 @@
         <v>323</v>
       </c>
       <c r="B6" s="6">
-        <v>4721.55</v>
+        <v>14721.55</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6" s="3"/>
     </row>

</xml_diff>